<commit_message>
add / correct alignment description
</commit_message>
<xml_diff>
--- a/Sylvia grid CLIQUES.xlsx
+++ b/Sylvia grid CLIQUES.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t>A6</t>
   </si>
@@ -150,7 +150,7 @@
     <t xml:space="preserve">Legend</t>
   </si>
   <si>
-    <t xml:space="preserve">* Positive construct poles (as indicated by column 'preferred') are aligned on the left</t>
+    <t xml:space="preserve">* Positive construct poles (as indicated by column 'preferred') are aligned on the right</t>
   </si>
   <si>
     <t xml:space="preserve">** 1 = positive relatedness, -1 = negative relatedness</t>
@@ -288,6 +288,9 @@
     <t xml:space="preserve">The minimal number of matching or inversely matching rating scores for two constructs to be considered 'related' has been set to 6.</t>
   </si>
   <si>
+    <t xml:space="preserve">Positive poles are right-aligned, i.e. the second pole of the construct is always the preferred pole.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Clique Nr.</t>
   </si>
   <si>
@@ -297,7 +300,7 @@
     <t xml:space="preserve">Label</t>
   </si>
   <si>
-    <t xml:space="preserve">Figure 1b: Network diagram for all constructs (full labels)</t>
+    <t xml:space="preserve">Figure 1a: Network diagram for all constructs (full labels)</t>
   </si>
   <si>
     <t xml:space="preserve">Lines represent relatedness of constructs</t>
@@ -306,13 +309,13 @@
     <t xml:space="preserve">Colored hull indicates a clique</t>
   </si>
   <si>
-    <t xml:space="preserve">Figure 2b: Network diagram for constructs inside cliques only (full labels)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Figure 1a: Network diagram for all constructs (construct no. as labels)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Figure 2a: Network diagram for constructs inside cliques only (construct no. as labels)</t>
+    <t xml:space="preserve">Figure 2a: Network diagram for constructs inside cliques only (full labels)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figure 1b: Network diagram for all constructs (construct no. as labels)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figure 2b: Network diagram for constructs inside cliques only (construct no. as labels)</t>
   </si>
 </sst>
 </file>
@@ -531,7 +534,7 @@
     <xdr:from xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
       <xdr:col xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:col>
       <xdr:colOff xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:colOff>
-      <xdr:row xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">34</xdr:row>
+      <xdr:row xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">35</xdr:row>
       <xdr:rowOff xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:rowOff>
     </xdr:from>
     <xdr:ext xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" cx="7200000" cy="7200000"/>
@@ -561,7 +564,7 @@
     <xdr:from xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
       <xdr:col xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">12</xdr:col>
       <xdr:colOff xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:colOff>
-      <xdr:row xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">34</xdr:row>
+      <xdr:row xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">35</xdr:row>
       <xdr:rowOff xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:rowOff>
     </xdr:from>
     <xdr:ext xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" cx="7200000" cy="7200000"/>
@@ -591,7 +594,7 @@
     <xdr:from xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
       <xdr:col xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:col>
       <xdr:colOff xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:colOff>
-      <xdr:row xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">79</xdr:row>
+      <xdr:row xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">80</xdr:row>
       <xdr:rowOff xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:rowOff>
     </xdr:from>
     <xdr:ext xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" cx="7200000" cy="7200000"/>
@@ -621,7 +624,7 @@
     <xdr:from xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
       <xdr:col xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">12</xdr:col>
       <xdr:colOff xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:colOff>
-      <xdr:row xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">79</xdr:row>
+      <xdr:row xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">80</xdr:row>
       <xdr:rowOff xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:rowOff>
     </xdr:from>
     <xdr:ext xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" cx="7200000" cy="7200000"/>
@@ -3308,31 +3311,19 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="9" t="s">
+    <row r="8">
+      <c r="A8" s="13" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" t="s">
-        <v>73</v>
-      </c>
-      <c r="D10" t="s">
-        <v>76</v>
-      </c>
-      <c r="E10" t="s">
-        <v>68</v>
+      <c r="A10" s="9" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" t="s">
         <v>75</v>
@@ -3344,162 +3335,171 @@
         <v>76</v>
       </c>
       <c r="E11" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
         <v>68</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>70</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>81</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="B14" s="9" t="s">
+    <row r="15">
+      <c r="A15" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="B15" s="9" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>1</v>
+      <c r="C15" s="9" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="16">
-      <c r="B16" t="s">
-        <v>75</v>
-      </c>
-      <c r="C16" t="s">
-        <v>57</v>
+      <c r="A16" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="s">
         <v>68</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>2</v>
-      </c>
-    </row>
     <row r="21">
-      <c r="B21" t="s">
-        <v>75</v>
-      </c>
-      <c r="C21" t="s">
-        <v>57</v>
+      <c r="A21" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="s">
         <v>72</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>3</v>
-      </c>
-    </row>
     <row r="26">
-      <c r="B26" t="s">
-        <v>68</v>
-      </c>
-      <c r="C26" t="s">
-        <v>50</v>
+      <c r="A26" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C28" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="s">
         <v>74</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="M31" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
     <row r="32">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="M32" s="13" t="s">
-        <v>94</v>
+      <c r="M32" s="9" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="33">
@@ -3510,20 +3510,20 @@
         <v>95</v>
       </c>
     </row>
-    <row r="76">
-      <c r="A76" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="M76" s="9" t="s">
+    <row r="34">
+      <c r="A34" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="M34" s="13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="9" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="77">
-      <c r="A77" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="M77" s="13" t="s">
-        <v>94</v>
+      <c r="M77" s="9" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="78">
@@ -3532,6 +3532,14 @@
       </c>
       <c r="M78" s="13" t="s">
         <v>95</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="M79" s="13" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>